<commit_message>
Add Treasury Project Manager Role Center extension
- Introduced a new page extension for the Treasury Project Manager Role Center.
- Added layout modifications to include Treasury Activities section.
- Implemented actions for managing Security Accounts, Securities, ISINs, and Treasury Setup.
- Enhanced user experience with tooltips and organized action groups.
</commit_message>
<xml_diff>
--- a/Security Management/.resources/Table list.xlsx
+++ b/Security Management/.resources/Table list.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,10 +413,16 @@
         <v>Name</v>
       </c>
       <c r="D1" t="str">
+        <v>Dansk titel</v>
+      </c>
+      <c r="E1" t="str">
         <v>Status</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Comments in ReadMe</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Stamdata</v>
       </c>
     </row>
     <row r="2">
@@ -430,9 +436,15 @@
         <v>Account</v>
       </c>
       <c r="D2" t="str">
+        <v>Depot</v>
+      </c>
+      <c r="E2" t="str">
         <v>Completed</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G2" t="str">
         <v>Yes</v>
       </c>
     </row>
@@ -446,6 +458,15 @@
       <c r="C3" t="str">
         <v>Security</v>
       </c>
+      <c r="D3" t="str">
+        <v>Værdipapir</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Completed for now</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -457,6 +478,12 @@
       <c r="C4" t="str">
         <v>Security Ledger Entry</v>
       </c>
+      <c r="D4" t="str">
+        <v>Værdipapirspost</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Completed</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -480,7 +507,13 @@
         <v>Security Account</v>
       </c>
       <c r="D6" t="str">
+        <v>Depotbeholdning</v>
+      </c>
+      <c r="E6" t="str">
         <v>Completed</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Yes</v>
       </c>
     </row>
     <row r="7">
@@ -493,6 +526,12 @@
       <c r="C7" t="str">
         <v>Security Account Ledger Entry</v>
       </c>
+      <c r="D7" t="str">
+        <v>Depotbeholdsningspost</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Completed</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -526,6 +565,12 @@
       <c r="C10" t="str">
         <v>Security Register</v>
       </c>
+      <c r="D10" t="str">
+        <v>Værdipapirjournal</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Security Register</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -537,6 +582,12 @@
       <c r="C11" t="str">
         <v>Security Setup</v>
       </c>
+      <c r="D11" t="str">
+        <v>Opsætning af Treasury</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -548,6 +599,12 @@
       <c r="C12" t="str">
         <v>Security Posting Group</v>
       </c>
+      <c r="D12" t="str">
+        <v>Værdipapirbogføringsgruppe</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -559,6 +616,9 @@
       <c r="C13" t="str">
         <v>Security Value Posting Group</v>
       </c>
+      <c r="G13" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -581,6 +641,15 @@
       <c r="C15" t="str">
         <v>Security Comment Line</v>
       </c>
+      <c r="D15" t="str">
+        <v>Værdipapirbemærkningslinje</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Completed</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -625,6 +694,15 @@
       <c r="C19" t="str">
         <v>Price</v>
       </c>
+      <c r="D19" t="str">
+        <v>Fondskurser</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Completed</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -636,7 +714,7 @@
       <c r="C20" t="str">
         <v>Payment Days Setup</v>
       </c>
-      <c r="D20" t="str">
+      <c r="E20" t="str">
         <v>Skip</v>
       </c>
     </row>
@@ -650,7 +728,7 @@
       <c r="C21" t="str">
         <v>Payment Day</v>
       </c>
-      <c r="D21" t="str">
+      <c r="E21" t="str">
         <v>Skip</v>
       </c>
     </row>
@@ -664,7 +742,7 @@
       <c r="C22" t="str">
         <v>Payment Code</v>
       </c>
-      <c r="D22" t="str">
+      <c r="E22" t="str">
         <v>Skip</v>
       </c>
     </row>
@@ -678,7 +756,7 @@
       <c r="C23" t="str">
         <v>ISIN-code</v>
       </c>
-      <c r="D23" t="str">
+      <c r="E23" t="str">
         <v>Commpleted</v>
       </c>
     </row>
@@ -750,7 +828,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add detailed profit and value ledger entries, along with security journal management features
- Introduced new tables and pages for managing detailed profit and value ledger entries.
- Added security journal management functionalities, including templates and batches.
- Implemented permissions for accessing detailed ledger entries and security journals.
- Enhanced user interface with new list pages for detailed profit and value ledger entries.
- Updated translations for new terms in Danish.
- Refactored existing permissionset to include new security journal features.
</commit_message>
<xml_diff>
--- a/Security Management/.resources/Table list.xlsx
+++ b/Security Management/.resources/Table list.xlsx
@@ -616,6 +616,9 @@
       <c r="C13" t="str">
         <v>Security Value Posting Group</v>
       </c>
+      <c r="D13" t="str">
+        <v>Værdipapirværdibogføringsgruppe</v>
+      </c>
       <c r="G13" t="str">
         <v>Yes</v>
       </c>
@@ -661,6 +664,9 @@
       <c r="C16" t="str">
         <v>Security Detailed Information</v>
       </c>
+      <c r="E16" t="str">
+        <v>Skip?</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -715,7 +721,7 @@
         <v>Payment Days Setup</v>
       </c>
       <c r="E20" t="str">
-        <v>Skip</v>
+        <v>Skip?</v>
       </c>
     </row>
     <row r="21">
@@ -729,7 +735,7 @@
         <v>Payment Day</v>
       </c>
       <c r="E21" t="str">
-        <v>Skip</v>
+        <v>Skip?</v>
       </c>
     </row>
     <row r="22">
@@ -743,7 +749,7 @@
         <v>Payment Code</v>
       </c>
       <c r="E22" t="str">
-        <v>Skip</v>
+        <v>Skip?</v>
       </c>
     </row>
     <row r="23">
@@ -754,7 +760,10 @@
         <v>94421</v>
       </c>
       <c r="C23" t="str">
-        <v>ISIN-code</v>
+        <v>ISIN</v>
+      </c>
+      <c r="D23" t="str">
+        <v>ISIN</v>
       </c>
       <c r="E23" t="str">
         <v>Commpleted</v>
@@ -773,6 +782,9 @@
       <c r="C24" t="str">
         <v>Detailed Value Ledger Entry</v>
       </c>
+      <c r="D24" t="str">
+        <v>Detaljeret værdipost</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -784,6 +796,9 @@
       <c r="C25" t="str">
         <v>Detailed Profit Ledger Entry</v>
       </c>
+      <c r="D25" t="str">
+        <v>Detaljeret afkastspost</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -795,6 +810,9 @@
       <c r="C26" t="str">
         <v>Approval Templates</v>
       </c>
+      <c r="E26" t="str">
+        <v>Skip?</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -806,6 +824,9 @@
       <c r="C27" t="str">
         <v>Approval Setup</v>
       </c>
+      <c r="E27" t="str">
+        <v>Skip?</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -817,6 +838,9 @@
       <c r="C28" t="str">
         <v>Approval Code</v>
       </c>
+      <c r="E28" t="str">
+        <v>Skip?</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -827,6 +851,9 @@
       </c>
       <c r="C29" t="str">
         <v>Application Area Line</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Skip?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>